<commit_message>
update the test case
</commit_message>
<xml_diff>
--- a/myapp/test/Test Case.xlsx
+++ b/myapp/test/Test Case.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10912"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandafeng/Documents/GitHub/CITS5206-Human-Movement/myapp/test/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7CA9E8-8316-7F46-B3AF-3CC9C6A9D44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9335"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="14120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="67">
   <si>
     <t>Functionality</t>
   </si>
@@ -200,19 +206,28 @@
   </si>
   <si>
     <t>App will collect user location data on the background. User can minimize the app but can not close it.</t>
+  </si>
+  <si>
+    <t>User fill in the information. User is receiving the correct form, and there is a submit buttom for them to submit the form.</t>
+  </si>
+  <si>
+    <t>Widget testing</t>
+  </si>
+  <si>
+    <t>https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/UserInfo_test.dart </t>
+  </si>
+  <si>
+    <t>Ying Feng</t>
+  </si>
+  <si>
+    <t>User get to the user information page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,7 +240,6 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -233,139 +247,17 @@
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,194 +282,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -585,268 +291,29 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
@@ -855,62 +322,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1168,32 +598,32 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.2222222222222" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1111111111111" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.1111111111111" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1111111111111" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6666666666667" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1111111111111" customWidth="1"/>
-    <col min="7" max="7" width="15.6666666666667" customWidth="1"/>
-    <col min="8" max="8" width="10.6666666666667" customWidth="1"/>
-    <col min="9" max="9" width="10.8888888888889" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +652,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="86.4" spans="1:9">
+    <row r="2" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1248,7 +678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" ht="28.8" spans="1:9">
+    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1261,7 +691,6 @@
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="1"/>
       <c r="F3" t="s">
         <v>14</v>
       </c>
@@ -1272,7 +701,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" ht="86.4" spans="1:9">
+    <row r="4" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1298,19 +727,41 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:9" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" ht="86.4" spans="1:7">
+      <c r="B5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1326,7 +777,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" ht="57.6" spans="1:9">
+    <row r="7" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -1350,7 +801,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" ht="57.6" spans="1:7">
+    <row r="8" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -1371,7 +822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="57.6" spans="1:7">
+    <row r="9" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1384,7 +835,6 @@
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1"/>
       <c r="F9" t="s">
         <v>14</v>
       </c>
@@ -1392,7 +842,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" ht="43.2" spans="1:9">
+    <row r="10" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -1415,7 +865,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" ht="86.4" spans="1:9">
+    <row r="11" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -1441,12 +891,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" ht="86.4" spans="1:9">
+    <row r="13" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1472,7 +922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" ht="86.4" spans="1:9">
+    <row r="14" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1495,7 +945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" ht="86.4" spans="1:9">
+    <row r="15" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>56</v>
       </c>
@@ -1518,7 +968,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" ht="43.2" spans="1:9">
+    <row r="16" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1543,15 +993,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/main_test.dart"/>
-    <hyperlink ref="E6" r:id="rId2" display="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/MarkerForm_test.dart"/>
-    <hyperlink ref="E4" r:id="rId3" display="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/setting_test.dart"/>
-    <hyperlink ref="E11" r:id="rId4" display="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/editLocation_test.dart"/>
-    <hyperlink ref="E13" r:id="rId1" display="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/main_test.dart"/>
-    <hyperlink ref="E14" r:id="rId1" display="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/main_test.dart" tooltip="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/main_test.dart"/>
-    <hyperlink ref="E15" r:id="rId1" display="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/main_test.dart" tooltip="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/main_test.dart"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E14" r:id="rId6" tooltip="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/main_test.dart" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E15" r:id="rId7" tooltip="https://github.com/Hanchooi/CITS5206-Human-Movement/blob/main/myapp/test/main_test.dart" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>